<commit_message>
Alteracoes no html 2 e no xlsx 2
</commit_message>
<xml_diff>
--- a/Pasta2.xlsx
+++ b/Pasta2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arauj\Documents\Arquivos para o git hub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\db1start\exercicioAula03\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>XLSX2</t>
+  </si>
+  <si>
+    <t>Alteração no xlsx2</t>
   </si>
 </sst>
 </file>
@@ -344,17 +347,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>